<commit_message>
Completed Reimbursement Unit creation, updation, deletion & duplicate check.
</commit_message>
<xml_diff>
--- a/reimbursement/src/main/resources/TestData/TestData.xlsx
+++ b/reimbursement/src/main/resources/TestData/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="ReimbUnits" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -48,7 +48,7 @@
     <t xml:space="preserve">AutoUnit1</t>
   </si>
   <si>
-    <t xml:space="preserve">Create Custom flow</t>
+    <t xml:space="preserve">Create Custom flow1</t>
   </si>
   <si>
     <t xml:space="preserve">AutoUnit1_Description</t>
@@ -60,6 +60,9 @@
     <t xml:space="preserve">AutoUnit2</t>
   </si>
   <si>
+    <t xml:space="preserve">Create Custom flow2</t>
+  </si>
+  <si>
     <t xml:space="preserve">AutoUnit2_Description</t>
   </si>
   <si>
@@ -72,24 +75,21 @@
     <t xml:space="preserve">GrpCompany</t>
   </si>
   <si>
-    <t xml:space="preserve">Units</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ApprovalFlow</t>
-  </si>
-  <si>
     <t xml:space="preserve">Currency</t>
   </si>
   <si>
-    <t xml:space="preserve">Body</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reimb Form auto1</t>
   </si>
   <si>
     <t xml:space="preserve">Wild1</t>
   </si>
   <si>
+    <t xml:space="preserve">//variables to be associated with enums/fixed values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//can be passed thru test data or config.ini file : Grp company: take mongo Id</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reimb Form auto2</t>
   </si>
   <si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t xml:space="preserve">location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">values</t>
   </si>
   <si>
     <t xml:space="preserve">uppercappu</t>
@@ -144,6 +141,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -166,6 +164,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -179,6 +178,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -186,12 +186,14 @@
       <color rgb="FF1C1C1C"/>
       <name val="DejaVu Sans Mono"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF1C1C1C"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -348,15 +350,15 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.82"/>
   </cols>
@@ -406,10 +408,10 @@
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -439,11 +441,11 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.53"/>
@@ -453,35 +455,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="E1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>21</v>
       </c>
     </row>
@@ -499,7 +500,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -512,19 +513,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.36328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="18.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -555,44 +556,40 @@
       <c r="I1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="D2" s="0" t="n">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>5</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>5</v>
+        <v>500</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>500</v>
+        <v>10</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="I2" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="J2" s="0" t="s">
-        <v>35</v>
+      <c r="I2" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>